<commit_message>
updated snack list generator
</commit_message>
<xml_diff>
--- a/Assets/01_mega_movie_fundraiser.xlsx
+++ b/Assets/01_mega_movie_fundraiser.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://masseyhighschoolnz-my.sharepoint.com/personal/jgottschalk_masseyhigh_school_nz/Documents/Projects/02_Tutorial_Answers/12_Advanced_Programming_Revisited/Mega_Movie_Fundraiser/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://masseyhighschoolnz-my.sharepoint.com/personal/jgottschalk_masseyhigh_school_nz/Documents/Projects/02_Tutorial_Answers/12_Advanced_Programming_Revisited/Mega_Movie_Fundraiser/Assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D4FBD971-4FDC-4C91-81B9-6BDFBEF8125C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="16" documentId="8_{D4FBD971-4FDC-4C91-81B9-6BDFBEF8125C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{93A7C7D9-9EB9-4710-A362-62F7F23F9AB6}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{31E039A0-BFD1-4590-9D50-EC525F3332F7}"/>
   </bookViews>
@@ -16,7 +16,8 @@
     <sheet name="Prices" sheetId="1" r:id="rId1"/>
     <sheet name="Ticket Sheet" sheetId="2" r:id="rId2"/>
     <sheet name="Ticket Price" sheetId="3" r:id="rId3"/>
-    <sheet name="snack_test_plan" sheetId="4" r:id="rId4"/>
+    <sheet name="Snack_plan_lists" sheetId="5" r:id="rId4"/>
+    <sheet name="snack_test_plan" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="54">
   <si>
     <t>Movie Fundraiser</t>
   </si>
@@ -326,7 +327,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -370,6 +371,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1425,7 +1429,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA9165A9-5B83-4D71-BD6C-7E67D68F207F}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
@@ -1525,11 +1529,129 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE430889-337A-48E9-B530-E46F37E43CC9}">
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="257" zoomScaleNormal="257" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="15" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="25">
+        <v>2</v>
+      </c>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25">
+        <v>1</v>
+      </c>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="23">
+        <v>0</v>
+      </c>
+      <c r="C3" s="23">
+        <v>0</v>
+      </c>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23">
+        <v>0</v>
+      </c>
+      <c r="F3" s="23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="25"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="25">
+        <v>1</v>
+      </c>
+      <c r="F4" s="25"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="23">
+        <v>1</v>
+      </c>
+      <c r="C5" s="23"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="25"/>
+      <c r="C6" s="25">
+        <v>1</v>
+      </c>
+      <c r="D6" s="25">
+        <v>1</v>
+      </c>
+      <c r="E6" s="25"/>
+      <c r="F6" s="25">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{797FFC9F-B42F-4CE2-BBA3-AA250D2C5317}">
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="147" zoomScaleNormal="147" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView zoomScale="147" zoomScaleNormal="147" workbookViewId="0">
+      <selection sqref="A1:F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Completed program including instructions
</commit_message>
<xml_diff>
--- a/Assets/01_mega_movie_fundraiser.xlsx
+++ b/Assets/01_mega_movie_fundraiser.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://masseyhighschoolnz-my.sharepoint.com/personal/jgottschalk_masseyhigh_school_nz/Documents/Projects/02_Tutorial_Answers/12_Advanced_Programming_Revisited/Mega_Movie_Fundraiser/Assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="108" documentId="8_{D4FBD971-4FDC-4C91-81B9-6BDFBEF8125C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{763F83AF-2ADE-4BE5-B1F0-C685562CED3A}"/>
+  <xr:revisionPtr revIDLastSave="118" documentId="8_{D4FBD971-4FDC-4C91-81B9-6BDFBEF8125C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{035DA963-9EEC-4C04-80FC-39E28B44A5D9}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="2" activeTab="7" xr2:uid="{31E039A0-BFD1-4590-9D50-EC525F3332F7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="1" xr2:uid="{31E039A0-BFD1-4590-9D50-EC525F3332F7}"/>
   </bookViews>
   <sheets>
     <sheet name="Prices" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="59">
   <si>
     <t>Movie Fundraiser</t>
   </si>
@@ -609,9 +609,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="8" fontId="0" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -619,6 +616,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="8" fontId="0" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -968,10 +968,10 @@
       <c r="C3" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="E3" s="61" t="s">
+      <c r="E3" s="64" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="61"/>
+      <c r="F3" s="64"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -1151,8 +1151,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41873174-3C06-4FAD-B97F-02F649204032}">
   <dimension ref="A1:P13"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection sqref="A1:L10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1163,10 +1163,11 @@
     <col min="6" max="6" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="3.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.28515625" hidden="1" customWidth="1"/>
     <col min="10" max="10" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="9.7109375" customWidth="1"/>
+    <col min="16" max="16" width="10.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -1216,7 +1217,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>21</v>
       </c>
@@ -1264,7 +1265,7 @@
         <v>5.8000000000000007</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -1309,7 +1310,7 @@
         <v>8.6</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>23</v>
       </c>
@@ -1351,7 +1352,7 @@
         <v>8.3874999999999993</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>24</v>
       </c>
@@ -1396,7 +1397,7 @@
         <v>8.65</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -1444,7 +1445,7 @@
         <v>9.5</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>26</v>
       </c>
@@ -1489,7 +1490,7 @@
         <v>3.95</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>27</v>
       </c>
@@ -1534,7 +1535,7 @@
         <v>9.3324999999999996</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>28</v>
       </c>
@@ -1579,7 +1580,7 @@
         <v>8.6</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -1633,7 +1634,7 @@
         <v>4</v>
       </c>
       <c r="E12">
-        <f t="shared" ref="E12:H12" si="7">SUM(E2:E10)</f>
+        <f t="shared" ref="E12:P12" si="7">SUM(E2:E10)</f>
         <v>3</v>
       </c>
       <c r="F12">
@@ -1648,6 +1649,34 @@
         <f t="shared" si="7"/>
         <v>5</v>
       </c>
+      <c r="I12">
+        <f t="shared" si="7"/>
+        <v>55.5</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="K12" s="2">
+        <f t="shared" si="7"/>
+        <v>2.35</v>
+      </c>
+      <c r="L12" s="2">
+        <f t="shared" si="7"/>
+        <v>145.35</v>
+      </c>
+      <c r="N12" s="10">
+        <f t="shared" si="7"/>
+        <v>42.5</v>
+      </c>
+      <c r="O12" s="10">
+        <f t="shared" si="7"/>
+        <v>29.07</v>
+      </c>
+      <c r="P12" s="10">
+        <f t="shared" si="7"/>
+        <v>71.569999999999993</v>
+      </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C13" s="3" t="s">
@@ -1657,16 +1686,12 @@
         <f>COUNTA(A2:A10)</f>
         <v>9</v>
       </c>
-      <c r="N13" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="P13" s="10">
-        <f>SUM(P2:P12)</f>
-        <v>71.569999999999993</v>
-      </c>
+      <c r="N13" s="3"/>
+      <c r="P13" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2828,7 +2853,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7CEF898-4DFC-458B-AE2C-55C3E035E0A6}">
   <dimension ref="A1:L18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="195" zoomScaleNormal="195" workbookViewId="0">
+    <sheetView topLeftCell="A9" zoomScale="195" zoomScaleNormal="195" workbookViewId="0">
       <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
@@ -2897,7 +2922,7 @@
       <c r="G2" s="33">
         <v>1</v>
       </c>
-      <c r="H2" s="62">
+      <c r="H2" s="61">
         <f>C2*2.5+D2*3+E2*4.5+F2*2+G2*3.25</f>
         <v>12.75</v>
       </c>
@@ -2932,7 +2957,7 @@
       <c r="G3" s="36">
         <v>0</v>
       </c>
-      <c r="H3" s="63">
+      <c r="H3" s="62">
         <f t="shared" ref="H3:H6" si="0">C3*2.5+D3*3+E3*4.5+F3*2+G3*3.25</f>
         <v>0</v>
       </c>
@@ -2961,7 +2986,7 @@
         <v>1</v>
       </c>
       <c r="G4" s="33"/>
-      <c r="H4" s="62">
+      <c r="H4" s="61">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
@@ -2992,7 +3017,7 @@
       <c r="G5" s="36">
         <v>1</v>
       </c>
-      <c r="H5" s="63">
+      <c r="H5" s="62">
         <f t="shared" si="0"/>
         <v>5.75</v>
       </c>
@@ -3025,7 +3050,7 @@
       <c r="G6" s="39">
         <v>3</v>
       </c>
-      <c r="H6" s="64">
+      <c r="H6" s="63">
         <f t="shared" si="0"/>
         <v>17.25</v>
       </c>

</xml_diff>